<commit_message>
remove random asterisks in front of some metadata columns messing up validation
</commit_message>
<xml_diff>
--- a/assets/sample_metadata/wastewater_biosample_template.xlsx
+++ b/assets/sample_metadata/wastewater_biosample_template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\02.scratch\ppox\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\01.scripts\tostadas\assets\sample_metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2E8A571-DFC0-4667-AA15-E97820499912}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF391BB9-27D8-4848-B752-B45FDEE6A644}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21840" yWindow="6410" windowWidth="20790" windowHeight="17800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NWSS_Metadata" sheetId="1" r:id="rId1"/>
@@ -1665,24 +1665,6 @@
     <t>collection_site_id</t>
   </si>
   <si>
-    <t>*ww_population</t>
-  </si>
-  <si>
-    <t>*ww_sample_matrix</t>
-  </si>
-  <si>
-    <t>*ww_sample_type</t>
-  </si>
-  <si>
-    <t>*ww_sample_duration</t>
-  </si>
-  <si>
-    <t>*ww_surv_target_1</t>
-  </si>
-  <si>
-    <t>*ww_surv_target_1_known_present</t>
-  </si>
-  <si>
     <t>public health surveillance community-level</t>
   </si>
   <si>
@@ -1765,6 +1747,24 @@
   </si>
   <si>
     <t>807536001-S1S1-R</t>
+  </si>
+  <si>
+    <t>ww_population</t>
+  </si>
+  <si>
+    <t>ww_sample_matrix</t>
+  </si>
+  <si>
+    <t>ww_sample_type</t>
+  </si>
+  <si>
+    <t>ww_sample_duration</t>
+  </si>
+  <si>
+    <t>ww_surv_target_1</t>
+  </si>
+  <si>
+    <t>ww_surv_target_1_known_present</t>
   </si>
 </sst>
 </file>
@@ -2124,13 +2124,13 @@
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2444,8 +2444,8 @@
   </sheetPr>
   <dimension ref="A1:DV41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="99" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="AR1" zoomScale="99" workbookViewId="0">
+      <selection activeCell="BD9" sqref="BD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
@@ -2462,7 +2462,14 @@
     <col min="15" max="15" width="15.81640625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="15.81640625" customWidth="1"/>
     <col min="17" max="18" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="19" max="105" width="13.453125" customWidth="1"/>
+    <col min="19" max="25" width="13.453125" customWidth="1"/>
+    <col min="26" max="26" width="14.6328125" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="13.453125" customWidth="1"/>
+    <col min="29" max="29" width="18.08984375" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="16.36328125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="13.453125" customWidth="1"/>
+    <col min="32" max="32" width="19.90625" bestFit="1" customWidth="1"/>
+    <col min="33" max="105" width="13.453125" customWidth="1"/>
     <col min="106" max="106" width="13.453125" bestFit="1" customWidth="1"/>
     <col min="107" max="107" width="24.453125" bestFit="1" customWidth="1"/>
     <col min="108" max="113" width="13.453125" bestFit="1" customWidth="1"/>
@@ -2491,7 +2498,7 @@
         <v>369</v>
       </c>
       <c r="BQ1" s="24" t="s">
-        <v>379</v>
+        <v>373</v>
       </c>
       <c r="BS1" s="31"/>
       <c r="BT1" s="31"/>
@@ -2511,7 +2518,7 @@
         <v>300</v>
       </c>
       <c r="C2" s="26" t="s">
-        <v>402</v>
+        <v>396</v>
       </c>
       <c r="D2" s="26" t="s">
         <v>301</v>
@@ -2580,7 +2587,7 @@
         <v>319</v>
       </c>
       <c r="Z2" s="36" t="s">
-        <v>371</v>
+        <v>399</v>
       </c>
       <c r="AA2" s="33" t="s">
         <v>320</v>
@@ -2589,16 +2596,16 @@
         <v>321</v>
       </c>
       <c r="AC2" s="36" t="s">
-        <v>372</v>
+        <v>400</v>
       </c>
       <c r="AD2" s="36" t="s">
-        <v>373</v>
+        <v>401</v>
       </c>
       <c r="AE2" s="33" t="s">
         <v>322</v>
       </c>
       <c r="AF2" s="36" t="s">
-        <v>374</v>
+        <v>402</v>
       </c>
       <c r="AG2" s="33" t="s">
         <v>323</v>
@@ -2670,10 +2677,10 @@
         <v>345</v>
       </c>
       <c r="BD2" s="36" t="s">
-        <v>375</v>
+        <v>403</v>
       </c>
       <c r="BE2" s="36" t="s">
-        <v>376</v>
+        <v>404</v>
       </c>
       <c r="BF2" s="33" t="s">
         <v>346</v>
@@ -2781,59 +2788,59 @@
     </row>
     <row r="3" spans="1:118" s="18" customFormat="1" ht="18.75" customHeight="1">
       <c r="A3" s="44" t="s">
-        <v>403</v>
+        <v>397</v>
       </c>
       <c r="B3" s="44" t="s">
-        <v>403</v>
+        <v>397</v>
       </c>
       <c r="C3" s="44" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>381</v>
+        <v>375</v>
       </c>
       <c r="E3" s="45"/>
       <c r="M3" s="20" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="N3" s="20" t="s">
         <v>358</v>
       </c>
-      <c r="O3" s="51">
+      <c r="O3" s="49">
         <v>45886</v>
       </c>
       <c r="Q3" s="18" t="s">
         <v>287</v>
       </c>
       <c r="R3" s="18" t="s">
-        <v>382</v>
+        <v>376</v>
       </c>
       <c r="S3" s="48"/>
       <c r="T3" s="20" t="s">
-        <v>386</v>
+        <v>380</v>
       </c>
       <c r="U3" s="20"/>
       <c r="V3" s="20" t="s">
-        <v>377</v>
+        <v>371</v>
       </c>
       <c r="W3" s="20" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
       <c r="X3" s="20">
         <v>1741289.4280000001</v>
       </c>
       <c r="Y3" s="20"/>
       <c r="Z3" s="20" t="s">
-        <v>388</v>
+        <v>382</v>
       </c>
       <c r="AA3" s="20" t="s">
-        <v>383</v>
+        <v>377</v>
       </c>
       <c r="AB3" s="20" t="s">
-        <v>384</v>
+        <v>378</v>
       </c>
       <c r="AC3" s="20" t="s">
-        <v>385</v>
+        <v>379</v>
       </c>
       <c r="AD3" s="20" t="s">
         <v>359</v>
@@ -2864,7 +2871,7 @@
         <v>1</v>
       </c>
       <c r="AN3" s="20" t="s">
-        <v>400</v>
+        <v>394</v>
       </c>
       <c r="AO3" s="20" t="s">
         <v>1</v>
@@ -2876,28 +2883,28 @@
         <v>1</v>
       </c>
       <c r="AR3" s="20" t="s">
-        <v>389</v>
+        <v>383</v>
       </c>
       <c r="AS3" s="20" t="s">
         <v>360</v>
       </c>
       <c r="AT3" s="20" t="s">
-        <v>390</v>
+        <v>384</v>
       </c>
       <c r="AU3" s="20" t="s">
-        <v>391</v>
+        <v>385</v>
       </c>
       <c r="AV3" s="20" t="s">
-        <v>392</v>
+        <v>386</v>
       </c>
       <c r="AW3" s="20">
         <v>105440000</v>
       </c>
       <c r="AX3" s="20" t="s">
-        <v>393</v>
+        <v>387</v>
       </c>
       <c r="AY3" s="20" t="s">
-        <v>394</v>
+        <v>388</v>
       </c>
       <c r="AZ3" s="20" t="s">
         <v>1</v>
@@ -2918,16 +2925,16 @@
         <v>362</v>
       </c>
       <c r="BF3" s="21" t="s">
-        <v>395</v>
+        <v>389</v>
       </c>
       <c r="BG3" s="21">
         <v>154560</v>
       </c>
       <c r="BH3" s="21" t="s">
-        <v>394</v>
+        <v>388</v>
       </c>
       <c r="BI3" s="20" t="s">
-        <v>396</v>
+        <v>390</v>
       </c>
       <c r="BJ3" s="20" t="s">
         <v>361</v>
@@ -2936,19 +2943,19 @@
         <v>154560</v>
       </c>
       <c r="BL3" s="20" t="s">
-        <v>394</v>
+        <v>388</v>
       </c>
       <c r="BM3" s="20" t="s">
-        <v>397</v>
+        <v>391</v>
       </c>
       <c r="BN3" s="20" t="s">
         <v>362</v>
       </c>
       <c r="BO3" s="20" t="s">
-        <v>398</v>
+        <v>392</v>
       </c>
       <c r="BP3" s="20" t="s">
-        <v>399</v>
+        <v>393</v>
       </c>
       <c r="BS3" s="22"/>
       <c r="BT3" s="22"/>
@@ -2969,7 +2976,7 @@
         <v>288</v>
       </c>
       <c r="CB3" s="18" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="CC3" s="18" t="s">
         <v>304</v>
@@ -6009,7 +6016,7 @@
   <sheetData>
     <row r="1" spans="1:31">
       <c r="A1" t="s">
-        <v>380</v>
+        <v>374</v>
       </c>
     </row>
     <row r="2" spans="1:31" ht="18.75" customHeight="1">
@@ -6233,8 +6240,8 @@
   <sheetData>
     <row r="1" spans="1:11" ht="18.75" customHeight="1">
       <c r="A1" s="1"/>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -6248,10 +6255,10 @@
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="50" t="s">
+      <c r="B2" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="50"/>
+      <c r="C2" s="51"/>
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
@@ -6265,10 +6272,10 @@
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="49" t="s">
+      <c r="B3" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="49"/>
+      <c r="C3" s="50"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
@@ -6282,10 +6289,10 @@
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="49" t="s">
+      <c r="B4" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="49"/>
+      <c r="C4" s="50"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
@@ -6299,10 +6306,10 @@
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="49" t="s">
+      <c r="B5" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="49"/>
+      <c r="C5" s="50"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -6316,10 +6323,10 @@
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="49" t="s">
+      <c r="B6" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="49"/>
+      <c r="C6" s="50"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -6333,10 +6340,10 @@
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="49" t="s">
+      <c r="B7" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="49"/>
+      <c r="C7" s="50"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
@@ -6350,10 +6357,10 @@
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="49" t="s">
+      <c r="B8" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="49"/>
+      <c r="C8" s="50"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
@@ -6367,10 +6374,10 @@
       <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="49" t="s">
+      <c r="B9" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="49"/>
+      <c r="C9" s="50"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
@@ -6384,10 +6391,10 @@
       <c r="A10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="49" t="s">
+      <c r="B10" s="50" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="49"/>
+      <c r="C10" s="50"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
@@ -6401,10 +6408,10 @@
       <c r="A11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="49" t="s">
+      <c r="B11" s="50" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="49"/>
+      <c r="C11" s="50"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
@@ -6418,10 +6425,10 @@
       <c r="A12" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="49" t="s">
+      <c r="B12" s="50" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="49"/>
+      <c r="C12" s="50"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
@@ -6435,10 +6442,10 @@
       <c r="A13" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="49" t="s">
+      <c r="B13" s="50" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="49"/>
+      <c r="C13" s="50"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
@@ -6452,10 +6459,10 @@
       <c r="A14" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="49" t="s">
+      <c r="B14" s="50" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="49"/>
+      <c r="C14" s="50"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
@@ -6469,10 +6476,10 @@
       <c r="A15" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="49" t="s">
+      <c r="B15" s="50" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="49"/>
+      <c r="C15" s="50"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
@@ -6486,10 +6493,10 @@
       <c r="A16" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B16" s="49" t="s">
+      <c r="B16" s="50" t="s">
         <v>29</v>
       </c>
-      <c r="C16" s="49"/>
+      <c r="C16" s="50"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
@@ -6503,10 +6510,10 @@
       <c r="A17" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B17" s="49" t="s">
+      <c r="B17" s="50" t="s">
         <v>31</v>
       </c>
-      <c r="C17" s="49"/>
+      <c r="C17" s="50"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
@@ -6520,10 +6527,10 @@
       <c r="A18" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B18" s="49" t="s">
+      <c r="B18" s="50" t="s">
         <v>33</v>
       </c>
-      <c r="C18" s="49"/>
+      <c r="C18" s="50"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
@@ -6537,10 +6544,10 @@
       <c r="A19" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B19" s="49" t="s">
+      <c r="B19" s="50" t="s">
         <v>35</v>
       </c>
-      <c r="C19" s="49"/>
+      <c r="C19" s="50"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
@@ -6554,10 +6561,10 @@
       <c r="A20" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B20" s="49" t="s">
+      <c r="B20" s="50" t="s">
         <v>37</v>
       </c>
-      <c r="C20" s="49"/>
+      <c r="C20" s="50"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
@@ -6571,10 +6578,10 @@
       <c r="A21" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B21" s="49" t="s">
+      <c r="B21" s="50" t="s">
         <v>39</v>
       </c>
-      <c r="C21" s="49"/>
+      <c r="C21" s="50"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
@@ -6588,10 +6595,10 @@
       <c r="A22" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B22" s="49" t="s">
+      <c r="B22" s="50" t="s">
         <v>41</v>
       </c>
-      <c r="C22" s="49"/>
+      <c r="C22" s="50"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
@@ -6605,10 +6612,10 @@
       <c r="A23" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B23" s="49" t="s">
+      <c r="B23" s="50" t="s">
         <v>43</v>
       </c>
-      <c r="C23" s="49"/>
+      <c r="C23" s="50"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
@@ -6622,10 +6629,10 @@
       <c r="A24" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B24" s="49" t="s">
+      <c r="B24" s="50" t="s">
         <v>45</v>
       </c>
-      <c r="C24" s="49"/>
+      <c r="C24" s="50"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
@@ -6835,10 +6842,10 @@
       <c r="A37" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B37" s="49" t="s">
+      <c r="B37" s="50" t="s">
         <v>67</v>
       </c>
-      <c r="C37" s="49"/>
+      <c r="C37" s="50"/>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
@@ -6850,8 +6857,8 @@
     </row>
     <row r="38" spans="1:11" ht="18.75" customHeight="1">
       <c r="A38" s="1"/>
-      <c r="B38" s="49"/>
-      <c r="C38" s="49"/>
+      <c r="B38" s="50"/>
+      <c r="C38" s="50"/>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
@@ -6865,10 +6872,10 @@
       <c r="A39" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="B39" s="50" t="s">
+      <c r="B39" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="C39" s="50"/>
+      <c r="C39" s="51"/>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
@@ -6882,10 +6889,10 @@
       <c r="A40" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B40" s="49" t="s">
+      <c r="B40" s="50" t="s">
         <v>70</v>
       </c>
-      <c r="C40" s="49"/>
+      <c r="C40" s="50"/>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
@@ -6899,10 +6906,10 @@
       <c r="A41" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B41" s="49" t="s">
+      <c r="B41" s="50" t="s">
         <v>72</v>
       </c>
-      <c r="C41" s="49"/>
+      <c r="C41" s="50"/>
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
@@ -6916,10 +6923,10 @@
       <c r="A42" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B42" s="49" t="s">
+      <c r="B42" s="50" t="s">
         <v>74</v>
       </c>
-      <c r="C42" s="49"/>
+      <c r="C42" s="50"/>
       <c r="D42" s="1"/>
       <c r="E42" s="1"/>
       <c r="F42" s="1"/>
@@ -6933,10 +6940,10 @@
       <c r="A43" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B43" s="49" t="s">
+      <c r="B43" s="50" t="s">
         <v>76</v>
       </c>
-      <c r="C43" s="49"/>
+      <c r="C43" s="50"/>
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
       <c r="F43" s="1"/>
@@ -6950,10 +6957,10 @@
       <c r="A44" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B44" s="49" t="s">
+      <c r="B44" s="50" t="s">
         <v>78</v>
       </c>
-      <c r="C44" s="49"/>
+      <c r="C44" s="50"/>
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
@@ -6967,10 +6974,10 @@
       <c r="A45" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B45" s="49" t="s">
+      <c r="B45" s="50" t="s">
         <v>80</v>
       </c>
-      <c r="C45" s="49"/>
+      <c r="C45" s="50"/>
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
       <c r="F45" s="1"/>
@@ -7014,10 +7021,10 @@
       <c r="A48" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B48" s="49" t="s">
+      <c r="B48" s="50" t="s">
         <v>83</v>
       </c>
-      <c r="C48" s="49"/>
+      <c r="C48" s="50"/>
       <c r="D48" s="1"/>
       <c r="E48" s="1"/>
       <c r="F48" s="1"/>
@@ -7029,8 +7036,8 @@
     </row>
     <row r="49" spans="1:11" ht="18.75" customHeight="1">
       <c r="A49" s="1"/>
-      <c r="B49" s="49"/>
-      <c r="C49" s="49"/>
+      <c r="B49" s="50"/>
+      <c r="C49" s="50"/>
       <c r="D49" s="1"/>
       <c r="E49" s="1"/>
       <c r="F49" s="1"/>
@@ -7044,10 +7051,10 @@
       <c r="A50" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="B50" s="49" t="s">
+      <c r="B50" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="C50" s="49"/>
+      <c r="C50" s="50"/>
       <c r="D50" s="1"/>
       <c r="E50" s="1"/>
       <c r="F50" s="1"/>
@@ -7061,10 +7068,10 @@
       <c r="A51" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B51" s="49" t="s">
+      <c r="B51" s="50" t="s">
         <v>86</v>
       </c>
-      <c r="C51" s="49"/>
+      <c r="C51" s="50"/>
       <c r="D51" s="1"/>
       <c r="E51" s="1"/>
       <c r="F51" s="1"/>
@@ -7078,10 +7085,10 @@
       <c r="A52" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B52" s="49" t="s">
+      <c r="B52" s="50" t="s">
         <v>88</v>
       </c>
-      <c r="C52" s="49"/>
+      <c r="C52" s="50"/>
       <c r="D52" s="1"/>
       <c r="E52" s="1"/>
       <c r="F52" s="1"/>
@@ -7095,10 +7102,10 @@
       <c r="A53" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B53" s="49" t="s">
+      <c r="B53" s="50" t="s">
         <v>90</v>
       </c>
-      <c r="C53" s="49"/>
+      <c r="C53" s="50"/>
       <c r="D53" s="1"/>
       <c r="E53" s="1"/>
       <c r="F53" s="1"/>
@@ -7112,10 +7119,10 @@
       <c r="A54" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B54" s="49" t="s">
+      <c r="B54" s="50" t="s">
         <v>92</v>
       </c>
-      <c r="C54" s="49"/>
+      <c r="C54" s="50"/>
       <c r="D54" s="1"/>
       <c r="E54" s="1"/>
       <c r="F54" s="1"/>
@@ -7129,10 +7136,10 @@
       <c r="A55" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B55" s="49" t="s">
+      <c r="B55" s="50" t="s">
         <v>94</v>
       </c>
-      <c r="C55" s="49"/>
+      <c r="C55" s="50"/>
       <c r="D55" s="1"/>
       <c r="E55" s="1"/>
       <c r="F55" s="1"/>
@@ -7146,10 +7153,10 @@
       <c r="A56" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B56" s="49" t="s">
+      <c r="B56" s="50" t="s">
         <v>96</v>
       </c>
-      <c r="C56" s="49"/>
+      <c r="C56" s="50"/>
       <c r="D56" s="1"/>
       <c r="E56" s="1"/>
       <c r="F56" s="1"/>
@@ -7163,10 +7170,10 @@
       <c r="A57" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B57" s="49" t="s">
+      <c r="B57" s="50" t="s">
         <v>98</v>
       </c>
-      <c r="C57" s="49"/>
+      <c r="C57" s="50"/>
       <c r="D57" s="1"/>
       <c r="E57" s="1"/>
       <c r="F57" s="1"/>
@@ -7180,10 +7187,10 @@
       <c r="A58" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B58" s="49" t="s">
+      <c r="B58" s="50" t="s">
         <v>100</v>
       </c>
-      <c r="C58" s="49"/>
+      <c r="C58" s="50"/>
       <c r="D58" s="1"/>
       <c r="E58" s="1"/>
       <c r="F58" s="1"/>
@@ -7197,10 +7204,10 @@
       <c r="A59" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B59" s="49" t="s">
+      <c r="B59" s="50" t="s">
         <v>102</v>
       </c>
-      <c r="C59" s="49"/>
+      <c r="C59" s="50"/>
       <c r="D59" s="1"/>
       <c r="E59" s="1"/>
       <c r="F59" s="1"/>
@@ -7214,10 +7221,10 @@
       <c r="A60" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="B60" s="49" t="s">
+      <c r="B60" s="50" t="s">
         <v>104</v>
       </c>
-      <c r="C60" s="49"/>
+      <c r="C60" s="50"/>
       <c r="D60" s="1"/>
       <c r="E60" s="1"/>
       <c r="F60" s="1"/>
@@ -7231,10 +7238,10 @@
       <c r="A61" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B61" s="49" t="s">
+      <c r="B61" s="50" t="s">
         <v>106</v>
       </c>
-      <c r="C61" s="49"/>
+      <c r="C61" s="50"/>
       <c r="D61" s="1"/>
       <c r="E61" s="1"/>
       <c r="F61" s="1"/>
@@ -7248,10 +7255,10 @@
       <c r="A62" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B62" s="49" t="s">
+      <c r="B62" s="50" t="s">
         <v>108</v>
       </c>
-      <c r="C62" s="49"/>
+      <c r="C62" s="50"/>
       <c r="D62" s="1"/>
       <c r="E62" s="1"/>
       <c r="F62" s="1"/>
@@ -7265,10 +7272,10 @@
       <c r="A63" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B63" s="49" t="s">
+      <c r="B63" s="50" t="s">
         <v>110</v>
       </c>
-      <c r="C63" s="49"/>
+      <c r="C63" s="50"/>
       <c r="D63" s="1"/>
       <c r="E63" s="1"/>
       <c r="F63" s="1"/>
@@ -7282,10 +7289,10 @@
       <c r="A64" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B64" s="49" t="s">
+      <c r="B64" s="50" t="s">
         <v>112</v>
       </c>
-      <c r="C64" s="49"/>
+      <c r="C64" s="50"/>
       <c r="D64" s="1"/>
       <c r="E64" s="1"/>
       <c r="F64" s="1"/>
@@ -7299,10 +7306,10 @@
       <c r="A65" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B65" s="49" t="s">
+      <c r="B65" s="50" t="s">
         <v>114</v>
       </c>
-      <c r="C65" s="49"/>
+      <c r="C65" s="50"/>
       <c r="D65" s="1"/>
       <c r="E65" s="1"/>
       <c r="F65" s="1"/>
@@ -7316,10 +7323,10 @@
       <c r="A66" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B66" s="49" t="s">
+      <c r="B66" s="50" t="s">
         <v>116</v>
       </c>
-      <c r="C66" s="49"/>
+      <c r="C66" s="50"/>
       <c r="D66" s="1"/>
       <c r="E66" s="1"/>
       <c r="F66" s="1"/>
@@ -7333,10 +7340,10 @@
       <c r="A67" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B67" s="49" t="s">
+      <c r="B67" s="50" t="s">
         <v>118</v>
       </c>
-      <c r="C67" s="49"/>
+      <c r="C67" s="50"/>
       <c r="D67" s="1"/>
       <c r="E67" s="1"/>
       <c r="F67" s="1"/>
@@ -7350,10 +7357,10 @@
       <c r="A68" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B68" s="49" t="s">
+      <c r="B68" s="50" t="s">
         <v>120</v>
       </c>
-      <c r="C68" s="49"/>
+      <c r="C68" s="50"/>
       <c r="D68" s="1"/>
       <c r="E68" s="1"/>
       <c r="F68" s="1"/>
@@ -7367,10 +7374,10 @@
       <c r="A69" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="B69" s="49" t="s">
+      <c r="B69" s="50" t="s">
         <v>122</v>
       </c>
-      <c r="C69" s="49"/>
+      <c r="C69" s="50"/>
       <c r="D69" s="1"/>
       <c r="E69" s="1"/>
       <c r="F69" s="1"/>
@@ -7384,10 +7391,10 @@
       <c r="A70" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="B70" s="49" t="s">
+      <c r="B70" s="50" t="s">
         <v>124</v>
       </c>
-      <c r="C70" s="49"/>
+      <c r="C70" s="50"/>
       <c r="D70" s="1"/>
       <c r="E70" s="1"/>
       <c r="F70" s="1"/>
@@ -7401,10 +7408,10 @@
       <c r="A71" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="B71" s="49" t="s">
+      <c r="B71" s="50" t="s">
         <v>126</v>
       </c>
-      <c r="C71" s="49"/>
+      <c r="C71" s="50"/>
       <c r="D71" s="1"/>
       <c r="E71" s="1"/>
       <c r="F71" s="1"/>
@@ -7418,10 +7425,10 @@
       <c r="A72" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B72" s="49" t="s">
+      <c r="B72" s="50" t="s">
         <v>128</v>
       </c>
-      <c r="C72" s="49"/>
+      <c r="C72" s="50"/>
       <c r="D72" s="1"/>
       <c r="E72" s="1"/>
       <c r="F72" s="1"/>
@@ -7435,10 +7442,10 @@
       <c r="A73" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="B73" s="49" t="s">
+      <c r="B73" s="50" t="s">
         <v>130</v>
       </c>
-      <c r="C73" s="49"/>
+      <c r="C73" s="50"/>
       <c r="D73" s="1"/>
       <c r="E73" s="1"/>
       <c r="F73" s="1"/>
@@ -7452,10 +7459,10 @@
       <c r="A74" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="B74" s="49" t="s">
+      <c r="B74" s="50" t="s">
         <v>132</v>
       </c>
-      <c r="C74" s="49"/>
+      <c r="C74" s="50"/>
       <c r="D74" s="1"/>
       <c r="E74" s="1"/>
       <c r="F74" s="1"/>
@@ -7469,10 +7476,10 @@
       <c r="A75" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="B75" s="49" t="s">
+      <c r="B75" s="50" t="s">
         <v>134</v>
       </c>
-      <c r="C75" s="49"/>
+      <c r="C75" s="50"/>
       <c r="D75" s="1"/>
       <c r="E75" s="1"/>
       <c r="F75" s="1"/>
@@ -7486,10 +7493,10 @@
       <c r="A76" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="B76" s="49" t="s">
+      <c r="B76" s="50" t="s">
         <v>136</v>
       </c>
-      <c r="C76" s="49"/>
+      <c r="C76" s="50"/>
       <c r="D76" s="1"/>
       <c r="E76" s="1"/>
       <c r="F76" s="1"/>
@@ -7503,10 +7510,10 @@
       <c r="A77" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="B77" s="49" t="s">
+      <c r="B77" s="50" t="s">
         <v>138</v>
       </c>
-      <c r="C77" s="49"/>
+      <c r="C77" s="50"/>
       <c r="D77" s="1"/>
       <c r="E77" s="1"/>
       <c r="F77" s="1"/>
@@ -8094,61 +8101,6 @@
     </row>
   </sheetData>
   <mergeCells count="63">
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="B61:C61"/>
-    <mergeCell ref="B62:C62"/>
-    <mergeCell ref="B63:C63"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="B69:C69"/>
     <mergeCell ref="B75:C75"/>
     <mergeCell ref="B76:C76"/>
     <mergeCell ref="B77:C77"/>
@@ -8157,6 +8109,61 @@
     <mergeCell ref="B72:C72"/>
     <mergeCell ref="B73:C73"/>
     <mergeCell ref="B74:C74"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="B69:C69"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="B61:C61"/>
+    <mergeCell ref="B62:C62"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
title is optional in metadata template
</commit_message>
<xml_diff>
--- a/assets/sample_metadata/wastewater_biosample_template.xlsx
+++ b/assets/sample_metadata/wastewater_biosample_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\01.scripts\tostadas\assets\sample_metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF391BB9-27D8-4848-B752-B45FDEE6A644}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34C59883-7D00-4218-836C-7866A8BABEE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2444,8 +2444,8 @@
   </sheetPr>
   <dimension ref="A1:DV41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AR1" zoomScale="99" workbookViewId="0">
-      <selection activeCell="BD9" sqref="BD9"/>
+    <sheetView tabSelected="1" zoomScale="99" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
@@ -2523,7 +2523,7 @@
       <c r="D2" s="26" t="s">
         <v>301</v>
       </c>
-      <c r="E2" s="26" t="s">
+      <c r="E2" s="32" t="s">
         <v>312</v>
       </c>
       <c r="F2" s="32" t="s">
@@ -8101,6 +8101,61 @@
     </row>
   </sheetData>
   <mergeCells count="63">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="B61:C61"/>
+    <mergeCell ref="B62:C62"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="B69:C69"/>
     <mergeCell ref="B75:C75"/>
     <mergeCell ref="B76:C76"/>
     <mergeCell ref="B77:C77"/>
@@ -8109,61 +8164,6 @@
     <mergeCell ref="B72:C72"/>
     <mergeCell ref="B73:C73"/>
     <mergeCell ref="B74:C74"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="B69:C69"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="B61:C61"/>
-    <mergeCell ref="B62:C62"/>
-    <mergeCell ref="B63:C63"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>